<commit_message>
Somewhat clean commit, after a long hiatus
</commit_message>
<xml_diff>
--- a/literature/Katz_MSM reasons for testing 2014-07-23.xlsx
+++ b/literature/Katz_MSM reasons for testing 2014-07-23.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="140" windowWidth="25000" windowHeight="12960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0">Sheet1!$A$1:$F$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1">Sheet2!$A$1:$B$12</definedName>
+    <definedName name="ExternalData_1" localSheetId="1">Sheet2!$B$1:$C$12</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Table of testingreason by yeardx</t>
   </si>
@@ -90,13 +95,41 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>could be new dx but not new exposure</t>
+  </si>
+  <si>
+    <t>3-6 months</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>DATA ARE KC MSM ONLY</t>
+  </si>
+  <si>
+    <t>Could also possibly find the diagnosis date of the partner (long-term)</t>
+  </si>
+  <si>
+    <t>2/2/15: "other" could incorporate other risk-based tests like "positive partner's condom broke",  "partner cheated"…David will send</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,13 +144,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,23 +181,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -460,20 +523,20 @@
       <selection activeCell="G4" sqref="G4:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -481,7 +544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3">
         <v>2010</v>
       </c>
@@ -498,7 +561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -518,7 +581,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -538,7 +601,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -558,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -578,7 +641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -598,7 +661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -618,7 +681,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -638,7 +701,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -658,7 +721,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -678,7 +741,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -698,7 +761,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -718,7 +781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -740,472 +803,627 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="9.140625" style="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="1"/>
+    <col min="5" max="5" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8">
         <v>2010</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8">
         <v>2011</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8">
         <v>2012</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8">
         <v>2013</v>
       </c>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>59</v>
       </c>
-      <c r="C3" s="3">
-        <f>B3/B12</f>
+      <c r="D3" s="2">
+        <f>C3/C12</f>
         <v>8.5880640465793301E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>14</v>
       </c>
-      <c r="E3" s="3">
-        <f>D3/D12</f>
+      <c r="F3" s="2">
+        <f>E3/E12</f>
         <v>6.4814814814814811E-2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>19</v>
       </c>
-      <c r="G3" s="3">
-        <f>F3/F12</f>
+      <c r="H3" s="2">
+        <f>G3/G12</f>
         <v>0.1</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>12</v>
       </c>
-      <c r="I3" s="3">
-        <f>H3/H12</f>
+      <c r="J3" s="2">
+        <f>I3/I12</f>
         <v>7.4534161490683232E-2</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>14</v>
       </c>
-      <c r="K3" s="3">
-        <f>J3/J12</f>
+      <c r="L3" s="2">
+        <f>K3/K12</f>
         <v>0.11666666666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>4</v>
       </c>
-      <c r="C4" s="3">
-        <f>B4/B12</f>
+      <c r="D4" s="2">
+        <f>C4/C12</f>
         <v>5.822416302765648E-3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="3">
-        <f>D4/D12</f>
+      <c r="F4" s="2">
+        <f>E4/E12</f>
         <v>4.6296296296296294E-3</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="3">
-        <f>F4/F12</f>
+      <c r="H4" s="2">
+        <f>G4/G12</f>
         <v>0</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>3</v>
       </c>
-      <c r="I4" s="3">
-        <f>H4/H12</f>
+      <c r="J4" s="2">
+        <f>I4/I12</f>
         <v>1.8633540372670808E-2</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>0</v>
       </c>
-      <c r="K4" s="3">
-        <f>J4/J12</f>
+      <c r="L4" s="2">
+        <f>K4/K12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>30</v>
       </c>
-      <c r="C5" s="3">
-        <f>B5/B12</f>
+      <c r="D5" s="2">
+        <f>C5/C12</f>
         <v>4.3668122270742356E-2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>6</v>
       </c>
-      <c r="E5" s="3">
-        <f>D5/D12</f>
+      <c r="F5" s="2">
+        <f>E5/E12</f>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>9</v>
       </c>
-      <c r="G5" s="3">
-        <f>F5/F12</f>
+      <c r="H5" s="2">
+        <f>G5/G12</f>
         <v>4.736842105263158E-2</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>8</v>
       </c>
-      <c r="I5" s="3">
-        <f>H5/H12</f>
+      <c r="J5" s="2">
+        <f>I5/I12</f>
         <v>4.9689440993788817E-2</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>7</v>
       </c>
-      <c r="K5" s="3">
-        <f>J5/J12</f>
+      <c r="L5" s="2">
+        <f>K5/K12</f>
         <v>5.8333333333333334E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:12">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
         <v>9</v>
       </c>
-      <c r="C6" s="3">
-        <f>B6/B12</f>
+      <c r="D6" s="2">
+        <f>C6/C12</f>
         <v>1.3100436681222707E-2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="3">
-        <f>D6/D12</f>
+      <c r="F6" s="2">
+        <f>E6/E12</f>
         <v>4.6296296296296294E-3</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="3">
-        <f>F6/F12</f>
+      <c r="H6" s="2">
+        <f>G6/G12</f>
         <v>1.5789473684210527E-2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>3</v>
       </c>
-      <c r="I6" s="3">
-        <f>H6/H12</f>
+      <c r="J6" s="2">
+        <f>I6/I12</f>
         <v>1.8633540372670808E-2</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>2</v>
       </c>
-      <c r="K6" s="3">
-        <f>J6/J12</f>
+      <c r="L6" s="2">
+        <f>K6/K12</f>
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>90</v>
       </c>
-      <c r="C7" s="3">
-        <f>B7/B12</f>
+      <c r="D7" s="2">
+        <f>C7/C12</f>
         <v>0.13100436681222707</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>29</v>
       </c>
-      <c r="E7" s="3">
-        <f>D7/D12</f>
+      <c r="F7" s="2">
+        <f>E7/E12</f>
         <v>0.13425925925925927</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>23</v>
       </c>
-      <c r="G7" s="3">
-        <f>F7/F12</f>
+      <c r="H7" s="2">
+        <f>G7/G12</f>
         <v>0.12105263157894737</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>21</v>
       </c>
-      <c r="I7" s="3">
-        <f>H7/H12</f>
+      <c r="J7" s="2">
+        <f>I7/I12</f>
         <v>0.13043478260869565</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>17</v>
       </c>
-      <c r="K7" s="3">
-        <f>J7/J12</f>
+      <c r="L7" s="2">
+        <f>K7/K12</f>
         <v>0.14166666666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:12">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>77</v>
       </c>
-      <c r="C8" s="3">
-        <f>B8/B12</f>
+      <c r="D8" s="2">
+        <f>C8/C12</f>
         <v>0.11208151382823872</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>22</v>
       </c>
-      <c r="E8" s="3">
-        <f>D8/D12</f>
+      <c r="F8" s="2">
+        <f>E8/E12</f>
         <v>0.10185185185185185</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>23</v>
       </c>
-      <c r="G8" s="3">
-        <f>F8/F12</f>
+      <c r="H8" s="2">
+        <f>G8/G12</f>
         <v>0.12105263157894737</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>21</v>
       </c>
-      <c r="I8" s="3">
-        <f>H8/H12</f>
+      <c r="J8" s="2">
+        <f>I8/I12</f>
         <v>0.13043478260869565</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>11</v>
       </c>
-      <c r="K8" s="3">
-        <f>J8/J12</f>
+      <c r="L8" s="2">
+        <f>K8/K12</f>
         <v>9.166666666666666E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:12">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>208</v>
       </c>
-      <c r="C9" s="3">
-        <f>B9/B12</f>
+      <c r="D9" s="2">
+        <f>C9/C12</f>
         <v>0.3027656477438137</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>77</v>
       </c>
-      <c r="E9" s="3">
-        <f>D9/D12</f>
+      <c r="F9" s="2">
+        <f>E9/E12</f>
         <v>0.35648148148148145</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>45</v>
       </c>
-      <c r="G9" s="3">
-        <f>F9/F12</f>
+      <c r="H9" s="2">
+        <f>G9/G12</f>
         <v>0.23684210526315788</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>51</v>
       </c>
-      <c r="I9" s="3">
-        <f>H9/H12</f>
+      <c r="J9" s="2">
+        <f>I9/I12</f>
         <v>0.31677018633540371</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>35</v>
       </c>
-      <c r="K9" s="3">
-        <f>J9/J12</f>
+      <c r="L9" s="2">
+        <f>K9/K12</f>
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>19</v>
       </c>
-      <c r="C10" s="3">
-        <f>B10/B12</f>
+      <c r="D10" s="2">
+        <f>C10/C12</f>
         <v>2.7656477438136828E-2</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>5</v>
       </c>
-      <c r="E10" s="3">
-        <f>D10/D12</f>
+      <c r="F10" s="2">
+        <f>E10/E12</f>
         <v>2.3148148148148147E-2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>6</v>
       </c>
-      <c r="G10" s="3">
-        <f>F10/F12</f>
+      <c r="H10" s="2">
+        <f>G10/G12</f>
         <v>3.1578947368421054E-2</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>4</v>
       </c>
-      <c r="I10" s="3">
-        <f>H10/H12</f>
+      <c r="J10" s="2">
+        <f>I10/I12</f>
         <v>2.4844720496894408E-2</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>4</v>
       </c>
-      <c r="K10" s="3">
-        <f>J10/J12</f>
+      <c r="L10" s="2">
+        <f>K10/K12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:12">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>191</v>
       </c>
-      <c r="C11" s="3">
-        <f>B11/B12</f>
+      <c r="D11" s="2">
+        <f>C11/C12</f>
         <v>0.27802037845705968</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>61</v>
       </c>
-      <c r="E11" s="3">
-        <f>D11/D12</f>
+      <c r="F11" s="2">
+        <f>E11/E12</f>
         <v>0.28240740740740738</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>62</v>
       </c>
-      <c r="G11" s="3">
-        <f>F11/F12</f>
+      <c r="H11" s="2">
+        <f>G11/G12</f>
         <v>0.32631578947368423</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>38</v>
       </c>
-      <c r="I11" s="3">
-        <f>H11/H12</f>
+      <c r="J11" s="2">
+        <f>I11/I12</f>
         <v>0.2360248447204969</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>30</v>
       </c>
-      <c r="K11" s="3">
-        <f>J11/J12</f>
+      <c r="L11" s="2">
+        <f>K11/K12</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="1">
-        <f>SUM(B3:B11)</f>
+      <c r="C12" s="1">
+        <f>SUM(C3:C11)</f>
         <v>687</v>
       </c>
-      <c r="D12" s="1">
-        <f>SUM(D3:D11)</f>
+      <c r="E12" s="1">
+        <f>SUM(E3:E11)</f>
         <v>216</v>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" ref="F12:J12" si="0">SUM(F3:F11)</f>
+      <c r="G12" s="1">
+        <f t="shared" ref="G12:K12" si="0">SUM(G3:G11)</f>
         <v>190</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <f t="shared" si="0"/>
         <v>161</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
+    <row r="14" spans="1:12">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5">
+        <f>SUM(D3:D6)</f>
+        <v>0.148471615720524</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" ref="E14:L14" si="1">SUM(E3:E6)</f>
+        <v>22</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.10185185185185186</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.16315789473684211</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.16149068322981366</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.19166666666666665</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="5">
+        <f>SUM(D7:D8,D10)</f>
+        <v>0.27074235807860264</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" ref="E15:L15" si="2">SUM(E7:E8,E10)</f>
+        <v>56</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="2"/>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="2"/>
+        <v>0.27368421052631581</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="5">
+        <f>SUM(D9,D11)</f>
+        <v>0.58078602620087338</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" ref="E16:L16" si="3">SUM(E9,E11)</f>
+        <v>138</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="3"/>
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="3"/>
+        <v>107</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="3"/>
+        <v>0.56315789473684208</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="3"/>
+        <v>0.55279503105590067</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="L16" s="5">
+        <f t="shared" si="3"/>
+        <v>0.54166666666666674</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1215,8 +1433,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>